<commit_message>
Getting ready for Lab 7 submission
</commit_message>
<xml_diff>
--- a/Test Plans/BakedGoods.xlsx
+++ b/Test Plans/BakedGoods.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>Kristina Frye</t>
   </si>
@@ -125,6 +124,9 @@
   </si>
   <si>
     <t>First item in listbox is selected. Modify button changes back to Modify. Add button changes back to Add</t>
+  </si>
+  <si>
+    <t>Tab order:  Name, Price, Inactive, listbox, Update, Add</t>
   </si>
 </sst>
 </file>
@@ -499,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +540,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="8" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>

</xml_diff>